<commit_message>
Enhance vehicle configuration and optimization logic
- Added max_customers_per_route parameter to VehicleConfig for route capacity management.
- Introduced large_request_threshold, ortools_target_utilization, and ortools_safe_utilization in WarehouseConfig for improved warehouse management.
- Updated CVRPConfig to use new first_solution_strategy and local_search_metaheuristic for better optimization.
- Implemented stop callback for max customers per route constraint in OR-Tools solver.
- Refined warehouse allocation logic to handle customer volume thresholds and optimize vehicle utilization.
- Improved interactive map generation with updated route details and markers.
</commit_message>
<xml_diff>
--- a/output/excel/warehouse_orders.xlsx
+++ b/output/excel/warehouse_orders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,53 +468,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1005369701</t>
+          <t>1007311001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>МИХАЙЛОВИ ТРЕЙД ООД</t>
+          <t>ЕВРОСТИКС ЕООД</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>890</v>
+        <v>435</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>42.73157,23.26128</t>
+          <t>42.66956517919332,23.38250309228897</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>42.73157</v>
+        <v>42.66956517919332</v>
       </c>
       <c r="F2" t="n">
-        <v>23.26128</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1005369701</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>МИХАЙЛОВИ ТРЕЙД ООД</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>890</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>42.73157,23.26128</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>42.73157</v>
-      </c>
-      <c r="F3" t="n">
-        <v>23.26128</v>
+        <v>23.38250309228897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor vehicle and warehouse management logic for improved optimization
- Enhanced VehicleType enum with additional vehicle types and detailed comments.
- Updated VehicleConfig and LocationConfig dataclasses with clearer descriptions and new parameters.
- Modified CVRPSolution to include dropped customers for better tracking of unserviced clients.
- Refined OR-Tools solver to handle sector penalties and improved distance callback logic.
- Removed deprecated debug_allocation script and integrated warehouse allocation directly into the solver.
- Added integration test for warehouse logic in OR-Tools to ensure proper functionality.
- Improved output handling for generating reports and interactive maps with updated data.
</commit_message>
<xml_diff>
--- a/output/excel/warehouse_orders.xlsx
+++ b/output/excel/warehouse_orders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,27 +468,131 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1007311001</t>
+          <t>1005726603</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ЕВРОСТИКС ЕООД</t>
+          <t>МС МАРКЕТ ЕООД</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>435</v>
+        <v>9</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>42.66956517919332,23.38250309228897</t>
+          <t>42.78312,23.50552</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>42.66956517919332</v>
+        <v>42.78312</v>
       </c>
       <c r="F2" t="n">
-        <v>23.38250309228897</v>
+        <v>23.50552</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1005931802</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ЕЛАЦИТЕ - МЕД АД</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>42.69358,24.01901</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>42.69358</v>
+      </c>
+      <c r="F3" t="n">
+        <v>24.01901</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1001030032</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>КОМЕ ООД</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>42.95998703256908,23.35085604339838</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>42.95998703256908</v>
+      </c>
+      <c r="F4" t="n">
+        <v>23.35085604339838</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1005789101</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ПАРТИ ФУУД ДЗЗД</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>42.69613,24.07431</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>42.69613</v>
+      </c>
+      <c r="F5" t="n">
+        <v>24.07431</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1007004101</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>КРАСИ КАН ЕООД</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>42.54143,23.49765</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>42.54143</v>
+      </c>
+      <c r="F6" t="n">
+        <v>23.49765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final simple solver. Need to implement center and internal zones
</commit_message>
<xml_diff>
--- a/output/excel/warehouse_orders.xlsx
+++ b/output/excel/warehouse_orders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,131 +468,105 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1005726603</t>
+          <t>1005300703</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>МС МАРКЕТ ЕООД</t>
+          <t>ПРЕСТИЖ - ВЕ 2015 ООД</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>130</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>42.78312,23.50552</t>
+          <t>42.82892,23.19246</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>42.78312</v>
+        <v>42.82892</v>
       </c>
       <c r="F2" t="n">
-        <v>23.50552</v>
+        <v>23.19246</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1005931802</t>
+          <t>1005560104</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ЕЛАЦИТЕ - МЕД АД</t>
+          <t>ДИМИТРОВ ТРЕЙД СЪРВИС ООД</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>145</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>42.69358,24.01901</t>
+          <t>42.66627,23.36354</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>42.69358</v>
+        <v>42.66627</v>
       </c>
       <c r="F3" t="n">
-        <v>24.01901</v>
+        <v>23.36354</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1001030032</t>
+          <t>1005491601</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>КОМЕ ООД</t>
+          <t>ДЕСИ СОФИЯ ЕООД</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>575</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>42.95998703256908,23.35085604339838</t>
+          <t>42.70893,23.38806</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>42.95998703256908</v>
+        <v>42.70893</v>
       </c>
       <c r="F4" t="n">
-        <v>23.35085604339838</v>
+        <v>23.38806</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1005789101</t>
+          <t>1005355601</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ПАРТИ ФУУД ДЗЗД</t>
+          <t>ПЕЦКА ИВАНОВА ЕТ</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>42.69613,24.07431</t>
+          <t>42.73325,23.25145</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>42.69613</v>
+        <v>42.73325</v>
       </c>
       <c r="F5" t="n">
-        <v>24.07431</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1007004101</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>КРАСИ КАН ЕООД</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>42.54143,23.49765</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>42.54143</v>
-      </c>
-      <c r="F6" t="n">
-        <v>23.49765</v>
+        <v>23.25145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>